<commit_message>
Bus 30 more loaded
</commit_message>
<xml_diff>
--- a/Nord.xlsx
+++ b/Nord.xlsx
@@ -437,7 +437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
@@ -1161,7 +1161,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>-0.72699999999999998</v>
+        <v>-8</v>
       </c>
       <c r="C32">
         <v>-0.238953</v>
@@ -1487,7 +1487,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>